<commit_message>
modified:   yahoo.xlsx 	modified:   yahoo_finance.ipynb 	modified:   yahoo_finance.py 	deleted:    yahoo_updated.xlsx
</commit_message>
<xml_diff>
--- a/yahoo.xlsx
+++ b/yahoo.xlsx
@@ -1,30 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nomad\VS_projects\Yahoo_Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757AC190-B060-4643-8860-5E26DA34D74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FE837C-B417-46D2-9101-E0330D65993B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12264" yWindow="1152" windowWidth="21888" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>msft</t>
   </si>
   <si>
+    <t>AAPL</t>
+  </si>
+  <si>
     <t>amzn</t>
   </si>
   <si>
@@ -40,12 +56,21 @@
     <t>Price</t>
   </si>
   <si>
+    <t>TrailingPE</t>
+  </si>
+  <si>
     <t>ForwardPE</t>
   </si>
   <si>
     <t>DilutedEPS</t>
   </si>
   <si>
+    <t>eqww</t>
+  </si>
+  <si>
+    <t>asdqwe</t>
+  </si>
+  <si>
     <t>Beta (5Y monthly)</t>
   </si>
   <si>
@@ -58,19 +83,37 @@
     <t>50 Day MA</t>
   </si>
   <si>
+    <t>XD</t>
+  </si>
+  <si>
     <t>200 Day MA</t>
   </si>
   <si>
+    <t>Dividend Rate</t>
+  </si>
+  <si>
     <t>Dividend Yield</t>
   </si>
   <si>
-    <t>Dividend Rate</t>
-  </si>
-  <si>
-    <t>TrailingPE</t>
-  </si>
-  <si>
-    <t>AAPL</t>
+    <t>qweqwe</t>
+  </si>
+  <si>
+    <t>XDDD</t>
+  </si>
+  <si>
+    <t>qeqweq</t>
+  </si>
+  <si>
+    <t>eqw</t>
+  </si>
+  <si>
+    <t>qweqwewq</t>
+  </si>
+  <si>
+    <t>eqweqw</t>
+  </si>
+  <si>
+    <t>^ this is a formula</t>
   </si>
 </sst>
 </file>
@@ -388,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,79 +442,125 @@
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <f>B4+C4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>